<commit_message>
continue running simulations and fix minor issues
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_monte_carlo_-1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_monte_carlo_-1.xlsx
@@ -4833,34 +4833,34 @@
         <v>1.771522592038193</v>
       </c>
       <c r="AJ25" t="n">
-        <v>27.4963281437613</v>
+        <v>27.49649073909455</v>
       </c>
       <c r="AK25" t="n">
         <v>0</v>
       </c>
       <c r="AL25" t="n">
-        <v>21.23693284310591</v>
+        <v>21.23693284310588</v>
       </c>
       <c r="AM25" t="n">
-        <v>151.0881872216595</v>
+        <v>151.0881872216437</v>
       </c>
       <c r="AN25" t="n">
-        <v>252.1883123953748</v>
+        <v>252.1883123953749</v>
       </c>
       <c r="AO25" t="n">
-        <v>264.2629739664656</v>
+        <v>264.2606278137627</v>
       </c>
       <c r="AP25" t="n">
         <v>1946698.052062165</v>
       </c>
       <c r="AQ25" t="n">
-        <v>3.33066907387547e-13</v>
+        <v>1.554312234475219e-13</v>
       </c>
       <c r="AR25" t="n">
-        <v>1.023571932383093</v>
+        <v>1.023571932383115</v>
       </c>
       <c r="AS25" t="n">
-        <v>1.942483634680015</v>
+        <v>1.942483634680056</v>
       </c>
       <c r="AT25" t="n">
         <v>0</v>
@@ -4869,7 +4869,7 @@
         <v>0</v>
       </c>
       <c r="AV25" t="n">
-        <v>0.06561096086575628</v>
+        <v>0.06561096086575766</v>
       </c>
       <c r="AW25" t="n">
         <v>0</v>
@@ -11098,34 +11098,34 @@
         <v>1.823090664530222</v>
       </c>
       <c r="AJ60" t="n">
-        <v>22.92243819816993</v>
+        <v>22.92269893677831</v>
       </c>
       <c r="AK60" t="n">
         <v>0</v>
       </c>
       <c r="AL60" t="n">
-        <v>21.25663788749154</v>
+        <v>21.2566378874904</v>
       </c>
       <c r="AM60" t="n">
-        <v>153.7924226835961</v>
+        <v>153.7924226836103</v>
       </c>
       <c r="AN60" t="n">
-        <v>252.1976947416919</v>
+        <v>252.1976947416917</v>
       </c>
       <c r="AO60" t="n">
-        <v>215.6106972217144</v>
+        <v>215.6083510689943</v>
       </c>
       <c r="AP60" t="n">
         <v>1376297.794811317</v>
       </c>
       <c r="AQ60" t="n">
-        <v>-2.220446049250313e-13</v>
+        <v>-1.110223024625157e-13</v>
       </c>
       <c r="AR60" t="n">
-        <v>1.004485279408226</v>
+        <v>1.004485279408249</v>
       </c>
       <c r="AS60" t="n">
-        <v>1.906261938996961</v>
+        <v>1.906261938997005</v>
       </c>
       <c r="AT60" t="n">
         <v>0</v>
@@ -11134,7 +11134,7 @@
         <v>0</v>
       </c>
       <c r="AV60" t="n">
-        <v>0.06438750641006728</v>
+        <v>0.0643875064100688</v>
       </c>
       <c r="AW60" t="n">
         <v>0</v>
@@ -12351,34 +12351,34 @@
         <v>1.740128872694422</v>
       </c>
       <c r="AJ67" t="n">
-        <v>25.45593130263118</v>
+        <v>25.45608834787822</v>
       </c>
       <c r="AK67" t="n">
         <v>0</v>
       </c>
       <c r="AL67" t="n">
-        <v>21.29996385232764</v>
+        <v>21.29996385232762</v>
       </c>
       <c r="AM67" t="n">
-        <v>151.4325170965373</v>
+        <v>151.4325170965365</v>
       </c>
       <c r="AN67" t="n">
-        <v>252.2199074372223</v>
+        <v>252.2199074372224</v>
       </c>
       <c r="AO67" t="n">
-        <v>254.5740938383334</v>
+        <v>254.5717476856163</v>
       </c>
       <c r="AP67" t="n">
         <v>1991717.854542145</v>
       </c>
       <c r="AQ67" t="n">
-        <v>-3.33066907387547e-14</v>
+        <v>1.110223024625157e-13</v>
       </c>
       <c r="AR67" t="n">
-        <v>1.017581459248267</v>
+        <v>1.017581459248268</v>
       </c>
       <c r="AS67" t="n">
-        <v>1.931115214288398</v>
+        <v>1.931115214288401</v>
       </c>
       <c r="AT67" t="n">
         <v>0</v>
@@ -12387,7 +12387,7 @@
         <v>0</v>
       </c>
       <c r="AV67" t="n">
-        <v>0.06522697153781391</v>
+        <v>0.06522697153781401</v>
       </c>
       <c r="AW67" t="n">
         <v>0</v>
@@ -12530,34 +12530,34 @@
         <v>1.316547312145139</v>
       </c>
       <c r="AJ68" t="n">
-        <v>22.79330396527732</v>
+        <v>22.7934753310609</v>
       </c>
       <c r="AK68" t="n">
         <v>0</v>
       </c>
       <c r="AL68" t="n">
-        <v>21.18655658493592</v>
+        <v>21.18655647218606</v>
       </c>
       <c r="AM68" t="n">
-        <v>150.9330186761636</v>
+        <v>150.9330269879786</v>
       </c>
       <c r="AN68" t="n">
-        <v>252.1631261736968</v>
+        <v>252.1631261729286</v>
       </c>
       <c r="AO68" t="n">
-        <v>268.4914857027401</v>
+        <v>268.4891337051561</v>
       </c>
       <c r="AP68" t="n">
-        <v>2215243.981408049</v>
+        <v>2215243.981408048</v>
       </c>
       <c r="AQ68" t="n">
-        <v>4.440892098500626e-14</v>
+        <v>-1.110223024625157e-13</v>
       </c>
       <c r="AR68" t="n">
-        <v>1.027088872793352</v>
+        <v>1.02708886609996</v>
       </c>
       <c r="AS68" t="n">
-        <v>1.949157908343585</v>
+        <v>1.949157895641199</v>
       </c>
       <c r="AT68" t="n">
         <v>0</v>
@@ -12566,7 +12566,7 @@
         <v>0</v>
       </c>
       <c r="AV68" t="n">
-        <v>0.0658363967460539</v>
+        <v>0.06583639631700744</v>
       </c>
       <c r="AW68" t="n">
         <v>0</v>
@@ -13067,34 +13067,34 @@
         <v>1.843512111204241</v>
       </c>
       <c r="AJ71" t="n">
-        <v>21.62465470417364</v>
+        <v>21.61322643037476</v>
       </c>
       <c r="AK71" t="n">
         <v>0</v>
       </c>
       <c r="AL71" t="n">
-        <v>21.14202081436435</v>
+        <v>21.128432041166</v>
       </c>
       <c r="AM71" t="n">
-        <v>152.9879619108517</v>
+        <v>153.1541112298194</v>
       </c>
       <c r="AN71" t="n">
-        <v>252.1873104548488</v>
+        <v>252.1836431734909</v>
       </c>
       <c r="AO71" t="n">
-        <v>240.4646269578802</v>
+        <v>240.4342864899607</v>
       </c>
       <c r="AP71" t="n">
-        <v>1845947.334148114</v>
+        <v>1845947.334148113</v>
       </c>
       <c r="AQ71" t="n">
-        <v>-5.551115123125783e-14</v>
+        <v>1.110223024625157e-13</v>
       </c>
       <c r="AR71" t="n">
-        <v>1.016987419893191</v>
+        <v>1.017276102949207</v>
       </c>
       <c r="AS71" t="n">
-        <v>1.929987876102303</v>
+        <v>1.930535724371857</v>
       </c>
       <c r="AT71" t="n">
         <v>0</v>
@@ -13103,7 +13103,7 @@
         <v>0</v>
       </c>
       <c r="AV71" t="n">
-        <v>0.06518889361515354</v>
+        <v>0.06520739819904417</v>
       </c>
       <c r="AW71" t="n">
         <v>0</v>
@@ -13783,34 +13783,34 @@
         <v>1.459341680506774</v>
       </c>
       <c r="AJ75" t="n">
-        <v>13.72193441950796</v>
+        <v>13.72216709464243</v>
       </c>
       <c r="AK75" t="n">
         <v>0</v>
       </c>
       <c r="AL75" t="n">
-        <v>21.24270635138966</v>
+        <v>21.24270327036172</v>
       </c>
       <c r="AM75" t="n">
-        <v>151.5612572447586</v>
+        <v>151.5618069334044</v>
       </c>
       <c r="AN75" t="n">
-        <v>252.1912024557868</v>
+        <v>252.191202430169</v>
       </c>
       <c r="AO75" t="n">
-        <v>256.9815113993905</v>
+        <v>256.9787301054462</v>
       </c>
       <c r="AP75" t="n">
         <v>2098071.428044324</v>
       </c>
       <c r="AQ75" t="n">
-        <v>0</v>
+        <v>4.440892098500626e-14</v>
       </c>
       <c r="AR75" t="n">
-        <v>1.02031951683908</v>
+        <v>1.020318913962142</v>
       </c>
       <c r="AS75" t="n">
-        <v>1.936311363081363</v>
+        <v>1.936310218971654</v>
       </c>
       <c r="AT75" t="n">
         <v>0</v>
@@ -13819,7 +13819,7 @@
         <v>0</v>
       </c>
       <c r="AV75" t="n">
-        <v>0.06540248102938502</v>
+        <v>0.06540244238497328</v>
       </c>
       <c r="AW75" t="n">
         <v>0</v>
@@ -13962,34 +13962,34 @@
         <v>1.451807716809732</v>
       </c>
       <c r="AJ76" t="n">
-        <v>13.90084414578748</v>
+        <v>13.90101442665431</v>
       </c>
       <c r="AK76" t="n">
         <v>0</v>
       </c>
       <c r="AL76" t="n">
-        <v>21.25029196898111</v>
+        <v>21.25029196898108</v>
       </c>
       <c r="AM76" t="n">
-        <v>152.109494242355</v>
+        <v>152.1094942423512</v>
       </c>
       <c r="AN76" t="n">
-        <v>252.194804588477</v>
+        <v>252.1948045884772</v>
       </c>
       <c r="AO76" t="n">
-        <v>246.2708266267174</v>
+        <v>246.2684804740029</v>
       </c>
       <c r="AP76" t="n">
-        <v>1799384.074193659</v>
+        <v>1799384.07419366</v>
       </c>
       <c r="AQ76" t="n">
-        <v>4.440892098500626e-14</v>
+        <v>-6.661338147750939e-14</v>
       </c>
       <c r="AR76" t="n">
-        <v>1.015881214825886</v>
+        <v>1.015881214825892</v>
       </c>
       <c r="AS76" t="n">
-        <v>1.927888575435825</v>
+        <v>1.927888575435837</v>
       </c>
       <c r="AT76" t="n">
         <v>0</v>
@@ -13998,7 +13998,7 @@
         <v>0</v>
       </c>
       <c r="AV76" t="n">
-        <v>0.0651179858703393</v>
+        <v>0.06511798587033969</v>
       </c>
       <c r="AW76" t="n">
         <v>0</v>
@@ -14141,22 +14141,22 @@
         <v>1.560523743778205</v>
       </c>
       <c r="AJ77" t="n">
-        <v>17.14272951404227</v>
+        <v>17.14292862826219</v>
       </c>
       <c r="AK77" t="n">
         <v>0</v>
       </c>
       <c r="AL77" t="n">
-        <v>21.22358207530764</v>
+        <v>21.22358207530763</v>
       </c>
       <c r="AM77" t="n">
-        <v>150.9410468660558</v>
+        <v>150.9410468660561</v>
       </c>
       <c r="AN77" t="n">
-        <v>252.1592430846749</v>
+        <v>252.159243084675</v>
       </c>
       <c r="AO77" t="n">
-        <v>267.5795667203398</v>
+        <v>267.5772205676225</v>
       </c>
       <c r="AP77" t="n">
         <v>2031806.020347561</v>
@@ -14165,10 +14165,10 @@
         <v>3.552713678800501e-13</v>
       </c>
       <c r="AR77" t="n">
-        <v>1.025355579227025</v>
+        <v>1.025355579227026</v>
       </c>
       <c r="AS77" t="n">
-        <v>1.945868550478087</v>
+        <v>1.945868550478088</v>
       </c>
       <c r="AT77" t="n">
         <v>0</v>
@@ -14177,7 +14177,7 @@
         <v>0</v>
       </c>
       <c r="AV77" t="n">
-        <v>0.06572529262845234</v>
+        <v>0.06572529262845235</v>
       </c>
       <c r="AW77" t="n">
         <v>0</v>
@@ -15036,34 +15036,34 @@
         <v>1.90054140345521</v>
       </c>
       <c r="AJ82" t="n">
-        <v>12.47493582717393</v>
+        <v>12.47510052319115</v>
       </c>
       <c r="AK82" t="n">
         <v>0</v>
       </c>
       <c r="AL82" t="n">
-        <v>21.26878734608701</v>
+        <v>21.26878734553368</v>
       </c>
       <c r="AM82" t="n">
-        <v>151.3883210266375</v>
+        <v>151.3883212645473</v>
       </c>
       <c r="AN82" t="n">
-        <v>252.2266639176629</v>
+        <v>252.2266639175988</v>
       </c>
       <c r="AO82" t="n">
-        <v>256.4715432653761</v>
+        <v>256.4691969488094</v>
       </c>
       <c r="AP82" t="n">
         <v>1868728.342310633</v>
       </c>
       <c r="AQ82" t="n">
-        <v>-5.551115123125783e-14</v>
+        <v>1.332267629550188e-13</v>
       </c>
       <c r="AR82" t="n">
-        <v>1.019394504190865</v>
+        <v>1.019394503901043</v>
       </c>
       <c r="AS82" t="n">
-        <v>1.934555920328213</v>
+        <v>1.934555919778205</v>
       </c>
       <c r="AT82" t="n">
         <v>0</v>
@@ -15072,7 +15072,7 @@
         <v>0</v>
       </c>
       <c r="AV82" t="n">
-        <v>0.06534318771863444</v>
+        <v>0.06534318770005687</v>
       </c>
       <c r="AW82" t="n">
         <v>0</v>
@@ -18079,34 +18079,34 @@
         <v>1.800647510722467</v>
       </c>
       <c r="AJ99" t="n">
-        <v>24.62968553247783</v>
+        <v>24.62985533341116</v>
       </c>
       <c r="AK99" t="n">
         <v>0</v>
       </c>
       <c r="AL99" t="n">
-        <v>21.33847508252818</v>
+        <v>21.33847508252817</v>
       </c>
       <c r="AM99" t="n">
-        <v>150.4932448468169</v>
+        <v>150.4932448468226</v>
       </c>
       <c r="AN99" t="n">
-        <v>252.2003654622343</v>
+        <v>252.2003654622344</v>
       </c>
       <c r="AO99" t="n">
-        <v>264.8557677780135</v>
+        <v>264.8534216252888</v>
       </c>
       <c r="AP99" t="n">
-        <v>1933311.53004506</v>
+        <v>1933311.530045059</v>
       </c>
       <c r="AQ99" t="n">
-        <v>3.552713678800501e-13</v>
+        <v>2.220446049250313e-14</v>
       </c>
       <c r="AR99" t="n">
-        <v>1.020706708566616</v>
+        <v>1.020706708566609</v>
       </c>
       <c r="AS99" t="n">
-        <v>1.937046156182295</v>
+        <v>1.937046156182282</v>
       </c>
       <c r="AT99" t="n">
         <v>0</v>
@@ -18115,7 +18115,7 @@
         <v>0</v>
       </c>
       <c r="AV99" t="n">
-        <v>0.06542730001912007</v>
+        <v>0.06542730001911966</v>
       </c>
       <c r="AW99" t="n">
         <v>0</v>

</xml_diff>